<commit_message>
Edit olx & sort date
</commit_message>
<xml_diff>
--- a/news.xlsx
+++ b/news.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,17 +582,17 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>01 May 2020</t>
+          <t>б/д</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>https://basnews.kz/ru/cat/news</t>
+          <t>https://www.facebook.com/mediazona.central.asia</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>Архивы Новости - Басты жаңалықтар - Basnews.kz.</t>
+          <t>Медиазона. Центральная Азия | Facebook</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>04 May 2020</t>
+          <t>б/д</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>https://zhaikpress.kz/ru/reg-service/itogi-vneshnego-analiza-korrupcionnyx-riskov-v-zko-territorialnoj-inspekcii-lesnogo-xozyajstva-zhivotnogo-mira/</t>
+          <t>https://www.kt.kz/rus/ecology/obmelenie_reki_zhayyk_kakie_mery_predlagaet_minekologii_rk_1377913788.html</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>Итоги внешнего анализа коррупционных рисков в ЗКО ...</t>
+          <t>Обмеление реки Жайык: какие меры предлагает ...</t>
         </is>
       </c>
     </row>
@@ -631,22 +631,22 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>05 May 2020</t>
+          <t>б/д</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>http://lit.lib.ru/u/uzhegow_genrih_nikolaewich/genrih-84.shtml</t>
+          <t>https://ecogosfond.kz/wp-content/uploads/2021/03/Nacdoklad-ITOG-rus-15.01.docx</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>Ужегов Генрих Николаевич Словарь рифм Ужегова Г. Буква ...</t>
+          <t>зеленой экономике» за 2017 - 2019 годы Нур-Султан, 2020</t>
         </is>
       </c>
     </row>
@@ -658,22 +658,22 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>19 May 2020</t>
+          <t>б/д</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>http://faolex.fao.org/docs/pdf/uzb196621.pdf</t>
+          <t>https://lacmus.life/feed.html</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>Закон Республики Узбекистан об охоте и охотничьем ...</t>
+          <t>Последние новости Волгограда - Lacmus.life</t>
         </is>
       </c>
     </row>
@@ -685,22 +685,22 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз балобанов</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>19 May 2020</t>
+          <t>б/д</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>https://interlawyer.com.ua/pticy-pod-ohranoy-konvencii-cites</t>
+          <t>https://colab.research.google.com/drive/13jXOlCpArV-lm4jZQ0VgOpj6nFBYrLAr</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>Птицы под охраной Конвенции CITES</t>
+          <t>MBART fairseq to HF.ipynb - Google Colaboratory “Colab”</t>
         </is>
       </c>
     </row>
@@ -712,22 +712,22 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз балобанов</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>20 May 2020</t>
+          <t>01 May 2020</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>https://interlawyer.com.ua/hishchnye-pticy-cites</t>
+          <t>https://basnews.kz/ru/cat/news</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>Хищные птицы CITES | Sunrise Legal Company</t>
+          <t>Архивы Новости - Басты жаңалықтар - Basnews.kz.</t>
         </is>
       </c>
     </row>
@@ -739,22 +739,22 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>контрабандный вывоз степных черепах</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>21 May 2020</t>
+          <t>04 May 2020</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>https://www.archaeolog.ru/media/books_ksia/ksia_114.pdf</t>
+          <t>https://zhaikpress.kz/ru/reg-service/itogi-vneshnego-analiza-korrupcionnyx-riskov-v-zko-territorialnoj-inspekcii-lesnogo-xozyajstva-zhivotnogo-mira/</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>Вып. 114 - Институт археологии РАН</t>
+          <t>Итоги внешнего анализа коррупционных рисков в ЗКО ...</t>
         </is>
       </c>
     </row>
@@ -771,17 +771,17 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>22 May 2020</t>
+          <t>05 May 2020</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>https://wwf.ru/resources/news/bioraznoobrazie/5-ugroz-biologicheskomu-raznoobraziyu-v-mire-posle-pandemii/</t>
+          <t>http://lit.lib.ru/u/uzhegow_genrih_nikolaewich/genrih-84.shtml</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>5 угроз биологическому разнообразию в мире после ...</t>
+          <t>Ужегов Генрих Николаевич Словарь рифм Ужегова Г. Буква ...</t>
         </is>
       </c>
     </row>
@@ -798,17 +798,17 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>27 May 2020</t>
+          <t>19 May 2020</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>https://www.kt.kz/rus/society/gde_v_almaty_mozhno_sdat_test_na_covid-19_1377899116.html</t>
+          <t>http://faolex.fao.org/docs/pdf/uzb196621.pdf</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>Где в Алматы можно сдать тест на COVID-19</t>
+          <t>Закон Республики Узбекистан об охоте и охотничьем ...</t>
         </is>
       </c>
     </row>
@@ -825,17 +825,17 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>27 May 2020</t>
+          <t>19 May 2020</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>https://www.s-vfu.ru/universitet/nauka/infao/ARCTIC%202035%202.pdf</t>
+          <t>https://interlawyer.com.ua/pticy-pod-ohranoy-konvencii-cites</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>АРКТИКА 2035 - СВФУ</t>
+          <t>Птицы под охраной Конвенции CITES</t>
         </is>
       </c>
     </row>
@@ -847,22 +847,22 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>31 May 2020</t>
+          <t>20 May 2020</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>https://kazpravda.kz/n/dobyvavshih-saygachi-roga-brakonerov-zaderzhali-v-zko/</t>
+          <t>https://interlawyer.com.ua/hishchnye-pticy-cites</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>Добывавших сайгачьи рога браконьеров задержали в ЗКО</t>
+          <t>Хищные птицы CITES | Sunrise Legal Company</t>
         </is>
       </c>
     </row>
@@ -879,17 +879,1826 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
+          <t>21 May 2020</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>https://www.archaeolog.ru/media/books_ksia/ksia_114.pdf</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>Вып. 114 - Институт археологии РАН</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="40" customHeight="1">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>22 May 2020</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>https://wwf.ru/resources/news/bioraznoobrazie/5-ugroz-biologicheskomu-raznoobraziyu-v-mire-posle-pandemii/</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>5 угроз биологическому разнообразию в мире после ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="40" customHeight="1">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>27 May 2020</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/society/gde_v_almaty_mozhno_sdat_test_na_covid-19_1377899116.html</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>Где в Алматы можно сдать тест на COVID-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="40" customHeight="1">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>27 May 2020</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>https://www.s-vfu.ru/universitet/nauka/infao/ARCTIC%202035%202.pdf</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>АРКТИКА 2035 - СВФУ</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="40" customHeight="1">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
           <t>31 May 2020</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>https://pcoding.ru/txt/words.txt</t>
-        </is>
-      </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>words.txt</t>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>https://kazpravda.kz/n/dobyvavshih-saygachi-roga-brakonerov-zaderzhali-v-zko/</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>Добывавших сайгачьи рога браконьеров задержали в ЗКО</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="40" customHeight="1">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>05 January 2021</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>https://kz.kursiv.media/2021-01-05/kak-ustroen-chernyy-rynok-saygachikh-rogov/</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>Как устроен черный рынок сайгачьих рогов - 05.01.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="40" customHeight="1">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>05 January 2021</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/DeepPavlov/rubert-base-cased-sentence/commit/5105dfa1852aa4da4c0ba0ba386bea565b1cc1f4.diff?file=0</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/DeepPavlov/rubert-base-case...</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="40" customHeight="1">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>18 January 2021</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>http://samlib.ru/b/bezbashennyj/antnarc10.shtml</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
+          <t>Безбашенный. Античная наркомафия - 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="40" customHeight="1">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>19 January 2021</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>https://www.osce.org/files/f/documents/5/e/338941.pdf</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>НАДЗОР ЗА ОБЪЕКТАМИ СИТЕС В ВОСТОЧНОЙ ЕВРОПЕ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="40" customHeight="1">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>22 January 2021</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/reviews/chto_budet_s_tsenami_na_myaso_v_2021_godu_1377910595.html</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>Что будет с ценами на мясо в 2021 году | Kazakhstan Today</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="40" customHeight="1">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>27 January 2021</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>https://mk-kz.kz/incident/2021/01/27/zakonodatelstvo-kazakhstana-ne-sposobno-protivostoyat-milliardam-nezakonnoy-pribyli-ot-brakonerstva.html</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="inlineStr">
+        <is>
+          <t>Законодательство Казахстана не способно противостоять ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="40" customHeight="1">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>29 January 2021</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>http://vch.ru/event/category/111.html?year=2021&amp;month=1</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>виртуальная таможня таможенно-логистический портал</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="40" customHeight="1">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>04 February 2021</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>https://www.gov.kz/uploads/2021/1/18/b045257d9841a8125edb6ec0b1efde4d_original.18115737.pdf</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
+          <t>Строительство МГ от УКПГ «Кашаган» до МГ «Макат ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="40" customHeight="1">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>19 February 2021</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>https://ved24.com/analytics/articles/2021-02-19/brakonerstvo-i-kontrabanda-chastey-derivatov-saygaka-zanesennogo-v</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
+          <t>Браконьерство и контрабанда частей (дериватов) сайгака ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="40" customHeight="1">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>07 March 2021</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>https://tengrinews.kz/kazakhstan_news/kazah-iz-kitaya-organizoval-kriminalnyiy-biznes-v-kazahstane-431007/</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="inlineStr">
+        <is>
+          <t>Казах из Китая организовал криминальный бизнес в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="40" customHeight="1">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>20 March 2021</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>http://www.nbpo.ru/wp-content/uploads/2021/01/%D0%A2%D0%91%D0%9E-%D0%A2%D0%9A%D0%9E-%D0%B4%D0%B5%D0%BA%D0%B0%D0%B1%D1%80%D1%8C-2020.doc</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="inlineStr">
+        <is>
+          <t>Заголовки</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="40" customHeight="1">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>30 March 2021</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>https://www.prozhito.org/memories?diaries=[6364]&amp;offset=150</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="inlineStr">
+        <is>
+          <t>Воспоминания - Прожито</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="40" customHeight="1">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>31 March 2021</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>http://corpus.leeds.ac.uk/frqc/internet-ru-doc.num</t>
+        </is>
+      </c>
+      <c r="E33" s="4" t="inlineStr">
+        <is>
+          <t>corpus.leeds.ac.uk/frqc/internet-ru-doc.num</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="40" customHeight="1">
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
+        <is>
+          <t>02 April 2021</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>https://matritca.kz/old/news/87420-uscherb-na-summu-14-mln-tenge-nanes-gosudarstvu-brakoner-iz-almatinskoy-oblasti.html</t>
+        </is>
+      </c>
+      <c r="E34" s="4" t="inlineStr">
+        <is>
+          <t>Ущерб на сумму 14 млн тенге нанес государству ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="40" customHeight="1">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>12 April 2021</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>https://liter.kz/na-2-mlrd-tenge-nashli-roga-sajgi-u-zhitelya-zko/</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
+          <t>Браконьеры из ЗКО хранили дома рога сайги на два ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="40" customHeight="1">
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
+        <is>
+          <t>12 April 2021</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kp.kz/online/news/4255453/</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="inlineStr">
+        <is>
+          <t>АО «НИТ» возглавил Ростислав Коняшкин - KP.Kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="40" customHeight="1">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="inlineStr">
+        <is>
+          <t>26 April 2021</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>https://guns.allzip.org/topic/250/2698262.html</t>
+        </is>
+      </c>
+      <c r="E37" s="4" t="inlineStr">
+        <is>
+          <t>Понемногу обо всем - 3 - Оружейный архив</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="40" customHeight="1">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>29 April 2021</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="inlineStr">
+        <is>
+          <t>https://elib.belstu.by/bitstream/123456789/39175/1/%D0%A0%D0%BE%D0%BC%D0%B0%D0%BD%D0%BE%D0%B2%20%D0%92.%20%D0%A1.%20-%20%D0%9E%D1%85%D0%BE%D1%82%D0%BE%D0%B2%D0%B5%D0%B4%D0%B5%D0%BD%D0%B8%D0%B5.pdf</t>
+        </is>
+      </c>
+      <c r="E38" s="4" t="inlineStr">
+        <is>
+          <t>Романов В. С. - Охотоведение.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="40" customHeight="1">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>05 May 2021</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>https://dknews.kz/ru/v-strane/181539-skolko-saygakov-ostalos-v-kazahstane-v-minekologii</t>
+        </is>
+      </c>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>Сколько сайгаков осталось в Казахстане - в Минэкологии ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="40" customHeight="1">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>05 May 2021</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>https://24.kz/ru/news/social/item/471950-5-maya-mezhdunarodnyj-den-sajgaka</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
+          <t>5 мая – Международный день сайгака - Хабар 24</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="40" customHeight="1">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>05 May 2021</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>https://qazaqtv.com/ru/news/society/8104-5-maya-mezhdunarodnyj-den-sajgaka</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
+          <t>5 мая – Международный день сайгака - QazaqTV</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="40" customHeight="1">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>08 May 2021</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>https://informburo.kz/sitemap/tags</t>
+        </is>
+      </c>
+      <c r="E42" s="4" t="inlineStr">
+        <is>
+          <t>Карта сайта: Теги | informburo.kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="40" customHeight="1">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="inlineStr">
+        <is>
+          <t>08 May 2021</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>https://naukaip.ru/wp-content/uploads/2021/01/%D0%9A-274.pdf</t>
+        </is>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
+          <t>ЛУЧШИЕ СТУДЕНЧЕСКИЕ ИССЛЕДОВАНИЯ</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="40" customHeight="1">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>17 May 2021</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>https://www.gov.kz/uploads/2021/5/17/97e8c6cbdb0d84db146a7858834ce060_original.4378435.pdf</t>
+        </is>
+      </c>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
+          <t>САПА КЕПІЛІ - GOV.KZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="40" customHeight="1">
+      <c r="A45" s="3" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="inlineStr">
+        <is>
+          <t>24 May 2021</t>
+        </is>
+      </c>
+      <c r="D45" s="3" t="inlineStr">
+        <is>
+          <t>https://rus.ozodlik.org/a/31270656.html</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>В Узбекистане задержаны браконьеры с 700 ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" ht="40" customHeight="1">
+      <c r="A46" s="3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>03 January 2022</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>https://goaravetisyan.ru/ekologiya-ostrov-sahalin-obyasnitelnaya-zapiska-2-detskie/</t>
+        </is>
+      </c>
+      <c r="E46" s="4" t="inlineStr">
+        <is>
+          <t>Экология остров сахалин. Объяснительная записка (2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="40" customHeight="1">
+      <c r="A47" s="3" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>05 January 2022</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/ecology/pravila_ucheta_domashnih_zhivotnyh_razrabotany_v_kazahstane_1377927178.html</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="inlineStr">
+        <is>
+          <t>Правила учета домашних животных разработаны в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="40" customHeight="1">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>07 January 2022</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>https://www.scribd.com/document/491297879/%D0%A1%D0%B5%D1%80%D0%B1%D1%81%D0%BA%D0%BE-%D0%A0%D1%83%D1%81%D1%81%D0%BA%D0%B8%D0%B9-%D1%81%D0%BB%D0%BE%D0%B2%D0%B0%D1%80%D1%8C-pdf</t>
+        </is>
+      </c>
+      <c r="E48" s="4" t="inlineStr">
+        <is>
+          <t>Сербско-Русский словарь PDF - Scribd</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" ht="40" customHeight="1">
+      <c r="A49" s="3" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="inlineStr">
+        <is>
+          <t>07 January 2022</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="inlineStr">
+        <is>
+          <t>https://ru.scribd.com/document/534658597/%D0%A7%D1%83%D0%B6%D0%BE%D0%B9-%D0%9D%D0%A0%D0%98-Core-rulebook</t>
+        </is>
+      </c>
+      <c r="E49" s="4" t="inlineStr">
+        <is>
+          <t>Чужой НРИ Core rulebook | PDF - Scribd</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" ht="40" customHeight="1">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>15 January 2022</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>https://www.rbc.ru/society/15/01/2022/61e257139a7947dd4fd28832</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="inlineStr">
+        <is>
+          <t>Росавиация установила причины экстренной посадки ... - РБК</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" ht="40" customHeight="1">
+      <c r="A51" s="3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="inlineStr">
+        <is>
+          <t>16 January 2022</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>https://zakon.uchet.kz/rus/docs/K1400000226</t>
+        </is>
+      </c>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>Уголовный кодекс Республики Казахстан</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" ht="40" customHeight="1">
+      <c r="A52" s="3" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B52" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>19 January 2022</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>http://forum-rybakov.ru/outfit/kachestvennye-i-funkcionalnye-seti-rybolovnye-obespechat-uvlekatelnoe-provedenie-dosuga-na-beregu-lyubogo-vodoema.html</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="inlineStr">
+        <is>
+          <t>Качественные и функциональные сети рыболовные ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" ht="40" customHeight="1">
+      <c r="A53" s="3" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>21 January 2022</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>https://newtimes.kz/obshchestvo/143464-v-petropavlovske-rasprodaiut-avtomobili-so-shtrafstoianki</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="inlineStr">
+        <is>
+          <t>В Петропавловске распродают автомобили со ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" ht="40" customHeight="1">
+      <c r="A54" s="3" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B54" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="inlineStr">
+        <is>
+          <t>21 January 2022</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>https://www.gov.kz/uploads/2022/1/21/195d4245b75123a2c2aecce3ed1ccb39_original.38998496.pdf</t>
+        </is>
+      </c>
+      <c r="E54" s="4" t="inlineStr">
+        <is>
+          <t>Национальный доклад о состоянии окружающей среды и ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" ht="40" customHeight="1">
+      <c r="A55" s="3" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="inlineStr">
+        <is>
+          <t>23 January 2022</t>
+        </is>
+      </c>
+      <c r="D55" s="3" t="inlineStr">
+        <is>
+          <t>http://samlib.ru/c/chernow_k_n/kp.shtml</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>Записки Империалиста Книга Вторая - Журнал "Самиздат"</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="40" customHeight="1">
+      <c r="A56" s="3" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="B56" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="inlineStr">
+        <is>
+          <t>05 July 2022</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="inlineStr">
+        <is>
+          <t>https://visasam.ru/russia/tamozhnia/vvoz-v-uzbekistan.html</t>
+        </is>
+      </c>
+      <c r="E56" s="4" t="inlineStr">
+        <is>
+          <t>Таможенные правила и пошлины Узбекистана в 2022 году</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" ht="40" customHeight="1">
+      <c r="A57" s="3" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="B57" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C57" s="3" t="inlineStr">
+        <is>
+          <t>06 July 2022</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="inlineStr">
+        <is>
+          <t>https://blog-rk.ru/simferopol/</t>
+        </is>
+      </c>
+      <c r="E57" s="4" t="inlineStr">
+        <is>
+          <t>Архивы Симферополь - Уютный Крым</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="40" customHeight="1">
+      <c r="A58" s="3" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B58" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="inlineStr">
+        <is>
+          <t>07 July 2022</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>https://blog-rk.ru/bez-rubriki/</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>Архивы Без рубрики - Уютный Крым</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" ht="40" customHeight="1">
+      <c r="A59" s="3" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="inlineStr">
+        <is>
+          <t>11 July 2022</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>https://baigenews.kz/news/ekoduki_ekspert_saygaki/</t>
+        </is>
+      </c>
+      <c r="E59" s="4" t="inlineStr">
+        <is>
+          <t>"На Западе экодуки строят даже для червей". Эксперт о ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" ht="40" customHeight="1">
+      <c r="A60" s="3" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C60" s="3" t="inlineStr">
+        <is>
+          <t>11 July 2022</t>
+        </is>
+      </c>
+      <c r="D60" s="3" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/sberbank-ai/sbert_large_nlu_ru/commit/6ef8561f2e0b07e4ef4d96ef5942c1c1c98efdab.diff</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>https://huggingface.co/sberbank-ai/sbert_large_nlu...</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" ht="40" customHeight="1">
+      <c r="A61" s="3" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B61" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C61" s="3" t="inlineStr">
+        <is>
+          <t>14 July 2022</t>
+        </is>
+      </c>
+      <c r="D61" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/reviews/vystuplenie_glavy_gosudarstva_kasym-zhomarta_tokaeva_na_1377936669.html</t>
+        </is>
+      </c>
+      <c r="E61" s="4" t="inlineStr">
+        <is>
+          <t>Выступление Главы государства Касым-Жомарта Токаева ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="40" customHeight="1">
+      <c r="A62" s="3" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="inlineStr">
+        <is>
+          <t>16 July 2022</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="inlineStr">
+        <is>
+          <t>https://dumskaya.net/wiki/edinoborstva/</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
+        <is>
+          <t>Единоборства, Одесса - новости, фото, биография ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="63" ht="40" customHeight="1">
+      <c r="A63" s="3" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="B63" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C63" s="3" t="inlineStr">
+        <is>
+          <t>19 July 2022</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="inlineStr">
+        <is>
+          <t>https://informburo.kz/stati/roga-i-kopyta-komu-byla-nuzhna-licenziya-na-unichtozhenie-80-tysyach-sajgakov</t>
+        </is>
+      </c>
+      <c r="E63" s="4" t="inlineStr">
+        <is>
+          <t>Рога и копыта: кому была нужна лицензия на уничтожение ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="40" customHeight="1">
+      <c r="A64" s="3" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="inlineStr">
+        <is>
+          <t>19 July 2022</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/crime/kontrabandnye_sigarety_na_527_3_mln_tenge_vyyavili_1377936914.html</t>
+        </is>
+      </c>
+      <c r="E64" s="4" t="inlineStr">
+        <is>
+          <t>Контрабандные сигареты на 527,3 млн тенге выявили ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" ht="40" customHeight="1">
+      <c r="A65" s="3" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B65" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C65" s="3" t="inlineStr">
+        <is>
+          <t>22 July 2022</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="inlineStr">
+        <is>
+          <t>https://flibusta.su/book/77996-velikiy-posledniy-shans-sbornik/read/</t>
+        </is>
+      </c>
+      <c r="E65" s="4" t="inlineStr">
+        <is>
+          <t>Великий последний шанс (сборник) читать онлайн ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="66" ht="40" customHeight="1">
+      <c r="A66" s="3" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B66" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C66" s="3" t="inlineStr">
+        <is>
+          <t>25 July 2022</t>
+        </is>
+      </c>
+      <c r="D66" s="3" t="inlineStr">
+        <is>
+          <t>http://minprom19.ru/o-ministerstve/novosti/?SHOWALL_1=1&amp;SIZEN_1=10</t>
+        </is>
+      </c>
+      <c r="E66" s="4" t="inlineStr">
+        <is>
+          <t>Новости - Министерство природных ресурсов и экологии</t>
+        </is>
+      </c>
+    </row>
+    <row r="67" ht="40" customHeight="1">
+      <c r="A67" s="3" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B67" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C67" s="3" t="inlineStr">
+        <is>
+          <t>25 July 2022</t>
+        </is>
+      </c>
+      <c r="D67" s="3" t="inlineStr">
+        <is>
+          <t>http://prezident.ov-russia.ru/</t>
+        </is>
+      </c>
+      <c r="E67" s="4" t="inlineStr">
+        <is>
+          <t>Президент РФ</t>
+        </is>
+      </c>
+    </row>
+    <row r="68" ht="40" customHeight="1">
+      <c r="A68" s="3" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B68" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C68" s="3" t="inlineStr">
+        <is>
+          <t>26 July 2022</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="inlineStr">
+        <is>
+          <t>https://ru.sputnik.kg/20220727/kazahstan-roga-sajga-izyatie-1066348561.html</t>
+        </is>
+      </c>
+      <c r="E68" s="4" t="inlineStr">
+        <is>
+          <t>В Казахстане в машине нашли 2 000 рогов сайги</t>
+        </is>
+      </c>
+    </row>
+    <row r="69" ht="40" customHeight="1">
+      <c r="A69" s="3" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="inlineStr">
+        <is>
+          <t>26 July 2022</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="inlineStr">
+        <is>
+          <t>https://mgorod.kz/nitem/roga-sajgakov-na-360-mln-tenge-obnaruzhili-v-avto-na-trasse-almaty-bishkek/</t>
+        </is>
+      </c>
+      <c r="E69" s="4" t="inlineStr">
+        <is>
+          <t>Рога сайгаков на 360 млн тенге обнаружили в авто на ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="70" ht="40" customHeight="1">
+      <c r="A70" s="3" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C70" s="3" t="inlineStr">
+        <is>
+          <t>26 July 2022</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="inlineStr">
+        <is>
+          <t>https://alarmyk24.ru/news/953564/pravitelstvo-rf-poddergalo-kostromskuyu-oblast-v-voprosah-raboty.html</t>
+        </is>
+      </c>
+      <c r="E70" s="4" t="inlineStr">
+        <is>
+          <t>Правительство РФ поддержало Костромскую область в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="71" ht="40" customHeight="1">
+      <c r="A71" s="3" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="B71" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C71" s="3" t="inlineStr">
+        <is>
+          <t>27 July 2022</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="inlineStr">
+        <is>
+          <t>https://zonakz.net/2022/07/27/pravitelstvo-podpisalo-razreshenie-na-vyvoz-bankami-rossijskix-rublej-iz-kazaxstana/</t>
+        </is>
+      </c>
+      <c r="E71" s="4" t="inlineStr">
+        <is>
+          <t>Правительство подписало разрешение на вывоз банками ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="72" ht="40" customHeight="1">
+      <c r="A72" s="3" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="inlineStr">
+        <is>
+          <t>27 July 2022</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="inlineStr">
+        <is>
+          <t>https://alarmyk24.ru/news/957532/reuters-byvshie-demokraty-i-respublikantsy-obyavili-o-sozdanii-tretej-partii-v-ssha.html</t>
+        </is>
+      </c>
+      <c r="E72" s="4" t="inlineStr">
+        <is>
+          <t>Reuters: бывшие демократы и республиканцы объявили о ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="73" ht="40" customHeight="1">
+      <c r="A73" s="3" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B73" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C73" s="3" t="inlineStr">
+        <is>
+          <t>28 July 2022</t>
+        </is>
+      </c>
+      <c r="D73" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/ecology/minekologii_raskritikovali_za_prodvizhenie_otstrela_saygi_1377937345.html</t>
+        </is>
+      </c>
+      <c r="E73" s="4" t="inlineStr">
+        <is>
+          <t>Минэкологии раскритиковали за продвижение отстрела ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="74" ht="40" customHeight="1">
+      <c r="A74" s="3" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B74" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
+        <is>
+          <t>28 July 2022</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="inlineStr">
+        <is>
+          <t>http://forum.guns.ru/forum_light_message_reverse/151/275304.html</t>
+        </is>
+      </c>
+      <c r="E74" s="4" t="inlineStr">
+        <is>
+          <t>Rom1983 : Бронежилет? Зачем? У кого какой? - Guns.ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="75" ht="40" customHeight="1">
+      <c r="A75" s="3" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B75" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C75" s="3" t="inlineStr">
+        <is>
+          <t>29 July 2022</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="inlineStr">
+        <is>
+          <t>https://liter.kz/roga-bolee-tysiachi-golov-saigi-obnaruzhili-u-brakonerov-v-almatinskoi-oblasti-1659080945/</t>
+        </is>
+      </c>
+      <c r="E75" s="4" t="inlineStr">
+        <is>
+          <t>Рога более тысячи голов сайги обнаружили у браконьеров ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="76" ht="40" customHeight="1">
+      <c r="A76" s="3" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B76" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C76" s="3" t="inlineStr">
+        <is>
+          <t>29 July 2022</t>
+        </is>
+      </c>
+      <c r="D76" s="3" t="inlineStr">
+        <is>
+          <t>https://coollib.net/b/279501-maksim-boyarinov-god-vorona-kniga-1-glavyi-1-32-si/read</t>
+        </is>
+      </c>
+      <c r="E76" s="4" t="inlineStr">
+        <is>
+          <t>Год ворона. Книга 1 (главы 1-32)(СИ) [Максим Бояринов ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" ht="40" customHeight="1">
+      <c r="A77" s="3" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="B77" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C77" s="3" t="inlineStr">
+        <is>
+          <t>30 July 2022</t>
+        </is>
+      </c>
+      <c r="D77" s="3" t="inlineStr">
+        <is>
+          <t>https://alarmyk24.ru/news/972416/yurist-rasskazal-v-kakih-sluchayah-u-vladeltsa-mogut-zabrat-avtomobil.html</t>
+        </is>
+      </c>
+      <c r="E77" s="4" t="inlineStr">
+        <is>
+          <t>Юрист рассказал, в каких случаях у владельца могут ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="78" ht="40" customHeight="1">
+      <c r="A78" s="3" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="B78" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="inlineStr">
+        <is>
+          <t>31 July 2022</t>
+        </is>
+      </c>
+      <c r="D78" s="3" t="inlineStr">
+        <is>
+          <t>https://ovu.com.ua/news-416366-pravitelstvo-razreshaet-torgovlyu-zapchastyami-regionam-porekomendovali-otkryt-servisy.html</t>
+        </is>
+      </c>
+      <c r="E78" s="4" t="inlineStr">
+        <is>
+          <t>Правительство разрешает торговлю запчастями ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="79" ht="40" customHeight="1">
+      <c r="A79" s="3" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C79" s="3" t="inlineStr">
+        <is>
+          <t>01 August 2022</t>
+        </is>
+      </c>
+      <c r="D79" s="3" t="inlineStr">
+        <is>
+          <t>https://polpred.com/news?ns=1&amp;cnt=69&amp;cat_a=1</t>
+        </is>
+      </c>
+      <c r="E79" s="4" t="inlineStr">
+        <is>
+          <t>Новости. Казахстан - Polpred.com Обзор СМИ</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" ht="40" customHeight="1">
+      <c r="A80" s="3" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="B80" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C80" s="3" t="inlineStr">
+        <is>
+          <t>02 August 2022</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/crime/_1377937567.html</t>
+        </is>
+      </c>
+      <c r="E80" s="4" t="inlineStr">
+        <is>
+          <t>В Алматы извращенца, пытавшегося изнасиловать дочь ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="81" ht="40" customHeight="1">
+      <c r="A81" s="3" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="inlineStr">
+        <is>
+          <t>03 August 2022</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="inlineStr">
+        <is>
+          <t>https://kazpravda.kz/</t>
+        </is>
+      </c>
+      <c r="E81" s="4" t="inlineStr">
+        <is>
+          <t>Новости Казахстана - свежие, актуальные, последние ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="82" ht="40" customHeight="1">
+      <c r="A82" s="3" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="B82" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C82" s="3" t="inlineStr">
+        <is>
+          <t>03 August 2022</t>
+        </is>
+      </c>
+      <c r="D82" s="3" t="inlineStr">
+        <is>
+          <t>https://xn--80ahclcogc6ci4h.xn--90anlfbebar6i.xn--p1ai/multimedia/photo/tags.htm?f=1&amp;blk=10407240&amp;objInBlock=24?</t>
+        </is>
+      </c>
+      <c r="E82" s="4" t="inlineStr">
+        <is>
+          <t>Фото по теме - Мультимедиа</t>
+        </is>
+      </c>
+    </row>
+    <row r="83" ht="40" customHeight="1">
+      <c r="A83" s="3" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="B83" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C83" s="3" t="inlineStr">
+        <is>
+          <t>03 August 2022</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="inlineStr">
+        <is>
+          <t>https://sibru.com/</t>
+        </is>
+      </c>
+      <c r="E83" s="4" t="inlineStr">
+        <is>
+          <t>SibRu.com | Новости Сибири</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add slanet, salazy, market
</commit_message>
<xml_diff>
--- a/news.xlsx
+++ b/news.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2170,22 +2170,22 @@
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>19 July 2022</t>
+          <t>16 July 2022</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
         <is>
-          <t>https://informburo.kz/stati/roga-i-kopyta-komu-byla-nuzhna-licenziya-na-unichtozhenie-80-tysyach-sajgakov</t>
+          <t>https://alashnews.kz/lenta</t>
         </is>
       </c>
       <c r="E64" s="4" t="inlineStr">
         <is>
-          <t>Рога и копыта: кому была нужна лицензия на уничтожение ...</t>
+          <t>Лента | Новости Казахстана - Alashnews</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>контрабанда сайгачьих рогов</t>
+          <t>контрабанда рогов сайгака</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
@@ -2207,12 +2207,12 @@
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>https://www.kt.kz/rus/crime/kontrabandnye_sigarety_na_527_3_mln_tenge_vyyavili_1377936914.html</t>
+          <t>https://informburo.kz/stati/roga-i-kopyta-komu-byla-nuzhna-licenziya-na-unichtozhenie-80-tysyach-sajgakov</t>
         </is>
       </c>
       <c r="E65" s="4" t="inlineStr">
         <is>
-          <t>Контрабандные сигареты на 527,3 млн тенге выявили ...</t>
+          <t>Рога и копыта: кому была нужна лицензия на уничтожение ...</t>
         </is>
       </c>
     </row>
@@ -2224,22 +2224,22 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>контрабандный вывоз степных черепах</t>
+          <t>контрабанда сайгачьих рогов</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>22 July 2022</t>
+          <t>19 July 2022</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
         <is>
-          <t>https://flibusta.su/book/77996-velikiy-posledniy-shans-sbornik/read/</t>
+          <t>https://www.kt.kz/rus/crime/kontrabandnye_sigarety_na_527_3_mln_tenge_vyyavili_1377936914.html</t>
         </is>
       </c>
       <c r="E66" s="4" t="inlineStr">
         <is>
-          <t>Великий последний шанс (сборник) читать онлайн ...</t>
+          <t>Контрабандные сигареты на 527,3 млн тенге выявили ...</t>
         </is>
       </c>
     </row>
@@ -2251,22 +2251,22 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз балобанов</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>25 July 2022</t>
+          <t>22 July 2022</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
         <is>
-          <t>http://minprom19.ru/o-ministerstve/novosti/?SHOWALL_1=1&amp;SIZEN_1=10</t>
+          <t>https://flibusta.su/book/77996-velikiy-posledniy-shans-sbornik/read/</t>
         </is>
       </c>
       <c r="E67" s="4" t="inlineStr">
         <is>
-          <t>Новости - Министерство природных ресурсов и экологии</t>
+          <t>Великий последний шанс (сборник) читать онлайн ...</t>
         </is>
       </c>
     </row>
@@ -2288,12 +2288,12 @@
       </c>
       <c r="D68" s="3" t="inlineStr">
         <is>
-          <t>http://prezident.ov-russia.ru/</t>
+          <t>http://minprom19.ru/o-ministerstve/novosti/?SHOWALL_1=1&amp;SIZEN_1=10</t>
         </is>
       </c>
       <c r="E68" s="4" t="inlineStr">
         <is>
-          <t>Президент РФ</t>
+          <t>Новости - Министерство природных ресурсов и экологии</t>
         </is>
       </c>
     </row>
@@ -2305,22 +2305,22 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>26 July 2022</t>
+          <t>25 July 2022</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
         <is>
-          <t>https://ru.sputnik.kg/20220727/kazahstan-roga-sajga-izyatie-1066348561.html</t>
+          <t>http://prezident.ov-russia.ru/</t>
         </is>
       </c>
       <c r="E69" s="4" t="inlineStr">
         <is>
-          <t>В Казахстане в машине нашли 2 000 рогов сайги</t>
+          <t>Президент РФ</t>
         </is>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабанда рогов сайгака</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -2342,12 +2342,12 @@
       </c>
       <c r="D70" s="3" t="inlineStr">
         <is>
-          <t>https://mgorod.kz/nitem/roga-sajgakov-na-360-mln-tenge-obnaruzhili-v-avto-na-trasse-almaty-bishkek/</t>
+          <t>https://ru.sputnik.kg/20220727/kazahstan-roga-sajga-izyatie-1066348561.html</t>
         </is>
       </c>
       <c r="E70" s="4" t="inlineStr">
         <is>
-          <t>Рога сайгаков на 360 млн тенге обнаружили в авто на ...</t>
+          <t>В Казахстане в машине нашли 2 000 рогов сайги</t>
         </is>
       </c>
     </row>
@@ -2369,12 +2369,12 @@
       </c>
       <c r="D71" s="3" t="inlineStr">
         <is>
-          <t>https://alarmyk24.ru/news/953564/pravitelstvo-rf-poddergalo-kostromskuyu-oblast-v-voprosah-raboty.html</t>
+          <t>https://mgorod.kz/nitem/roga-sajgakov-na-360-mln-tenge-obnaruzhili-v-avto-na-trasse-almaty-bishkek/</t>
         </is>
       </c>
       <c r="E71" s="4" t="inlineStr">
         <is>
-          <t>Правительство РФ поддержало Костромскую область в ...</t>
+          <t>Рога сайгаков на 360 млн тенге обнаружили в авто на ...</t>
         </is>
       </c>
     </row>
@@ -2391,17 +2391,17 @@
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>27 July 2022</t>
+          <t>26 July 2022</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
         <is>
-          <t>https://zonakz.net/2022/07/27/pravitelstvo-podpisalo-razreshenie-na-vyvoz-bankami-rossijskix-rublej-iz-kazaxstana/</t>
+          <t>https://alarmyk24.ru/news/953564/pravitelstvo-rf-poddergalo-kostromskuyu-oblast-v-voprosah-raboty.html</t>
         </is>
       </c>
       <c r="E72" s="4" t="inlineStr">
         <is>
-          <t>Правительство подписало разрешение на вывоз банками ...</t>
+          <t>Правительство РФ поддержало Костромскую область в ...</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз балобанов</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -2423,12 +2423,12 @@
       </c>
       <c r="D73" s="3" t="inlineStr">
         <is>
-          <t>https://alarmyk24.ru/news/957532/reuters-byvshie-demokraty-i-respublikantsy-obyavili-o-sozdanii-tretej-partii-v-ssha.html</t>
+          <t>https://zonakz.net/2022/07/27/pravitelstvo-podpisalo-razreshenie-na-vyvoz-bankami-rossijskix-rublej-iz-kazaxstana/</t>
         </is>
       </c>
       <c r="E73" s="4" t="inlineStr">
         <is>
-          <t>Reuters: бывшие демократы и республиканцы объявили о ...</t>
+          <t>Правительство подписало разрешение на вывоз банками ...</t>
         </is>
       </c>
     </row>
@@ -2440,22 +2440,22 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>28 July 2022</t>
+          <t>27 July 2022</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
         <is>
-          <t>https://www.kt.kz/rus/ecology/minekologii_raskritikovali_za_prodvizhenie_otstrela_saygi_1377937345.html</t>
+          <t>https://alarmyk24.ru/news/957532/reuters-byvshie-demokraty-i-respublikantsy-obyavili-o-sozdanii-tretej-partii-v-ssha.html</t>
         </is>
       </c>
       <c r="E74" s="4" t="inlineStr">
         <is>
-          <t>Минэкологии раскритиковали за продвижение отстрела ...</t>
+          <t>Reuters: бывшие демократы и республиканцы объявили о ...</t>
         </is>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>контрабандный вывоз степных черепах</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -2477,12 +2477,12 @@
       </c>
       <c r="D75" s="3" t="inlineStr">
         <is>
-          <t>http://forum.guns.ru/forum_light_message_reverse/151/275304.html</t>
+          <t>https://www.kt.kz/rus/ecology/minekologii_raskritikovali_za_prodvizhenie_otstrela_saygi_1377937345.html</t>
         </is>
       </c>
       <c r="E75" s="4" t="inlineStr">
         <is>
-          <t>Rom1983 : Бронежилет? Зачем? У кого какой? - Guns.ru</t>
+          <t>Минэкологии раскритиковали за продвижение отстрела ...</t>
         </is>
       </c>
     </row>
@@ -2494,22 +2494,22 @@
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>29 July 2022</t>
+          <t>28 July 2022</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
         <is>
-          <t>https://liter.kz/roga-bolee-tysiachi-golov-saigi-obnaruzhili-u-brakonerov-v-almatinskoi-oblasti-1659080945/</t>
+          <t>http://forum.guns.ru/forum_light_message_reverse/151/275304.html</t>
         </is>
       </c>
       <c r="E76" s="4" t="inlineStr">
         <is>
-          <t>Рога более тысячи голов сайги обнаружили у браконьеров ...</t>
+          <t>Rom1983 : Бронежилет? Зачем? У кого какой? - Guns.ru</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>контрабандный вывоз степных черепах</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
@@ -2531,12 +2531,12 @@
       </c>
       <c r="D77" s="3" t="inlineStr">
         <is>
-          <t>https://coollib.net/b/279501-maksim-boyarinov-god-vorona-kniga-1-glavyi-1-32-si/read</t>
+          <t>https://liter.kz/roga-bolee-tysiachi-golov-saigi-obnaruzhili-u-brakonerov-v-almatinskoi-oblasti-1659080945/</t>
         </is>
       </c>
       <c r="E77" s="4" t="inlineStr">
         <is>
-          <t>Год ворона. Книга 1 (главы 1-32)(СИ) [Максим Бояринов ...</t>
+          <t>Рога более тысячи голов сайги обнаружили у браконьеров ...</t>
         </is>
       </c>
     </row>
@@ -2548,22 +2548,22 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз балобанов</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>30 July 2022</t>
+          <t>29 July 2022</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
         <is>
-          <t>https://alarmyk24.ru/news/972416/yurist-rasskazal-v-kakih-sluchayah-u-vladeltsa-mogut-zabrat-avtomobil.html</t>
+          <t>https://coollib.net/b/279501-maksim-boyarinov-god-vorona-kniga-1-glavyi-1-32-si/read</t>
         </is>
       </c>
       <c r="E78" s="4" t="inlineStr">
         <is>
-          <t>Юрист рассказал, в каких случаях у владельца могут ...</t>
+          <t>Год ворона. Книга 1 (главы 1-32)(СИ) [Максим Бояринов ...</t>
         </is>
       </c>
     </row>
@@ -2575,22 +2575,22 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>31 July 2022</t>
+          <t>30 July 2022</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
         <is>
-          <t>https://ovu.com.ua/news-416366-pravitelstvo-razreshaet-torgovlyu-zapchastyami-regionam-porekomendovali-otkryt-servisy.html</t>
+          <t>https://alarmyk24.ru/news/972416/yurist-rasskazal-v-kakih-sluchayah-u-vladeltsa-mogut-zabrat-avtomobil.html</t>
         </is>
       </c>
       <c r="E79" s="4" t="inlineStr">
         <is>
-          <t>Правительство разрешает торговлю запчастями ...</t>
+          <t>Юрист рассказал, в каких случаях у владельца могут ...</t>
         </is>
       </c>
     </row>
@@ -2602,22 +2602,22 @@
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>контрабандный вывоз степных черепах</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>31 July 2022</t>
+          <t>30 July 2022</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
         <is>
-          <t>https://vk.com/wall-9029295</t>
+          <t>https://zonakz.net/2022/07/30/ceny-na-muku-i-luk-zamorozili-v-kostanajskoj-oblasti/</t>
         </is>
       </c>
       <c r="E80" s="4" t="inlineStr">
         <is>
-          <t>Европейской степи: записи сообщества | ВКонтакте</t>
+          <t>Цены на муку и лук заморозили в Костанайской области</t>
         </is>
       </c>
     </row>
@@ -2634,17 +2634,17 @@
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>01 August 2022</t>
+          <t>31 July 2022</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
         <is>
-          <t>https://polpred.com/news?ns=1&amp;cnt=69&amp;cat_a=1</t>
+          <t>https://ovu.com.ua/news-416366-pravitelstvo-razreshaet-torgovlyu-zapchastyami-regionam-porekomendovali-otkryt-servisy.html</t>
         </is>
       </c>
       <c r="E81" s="4" t="inlineStr">
         <is>
-          <t>Новости. Казахстан - Polpred.com Обзор СМИ</t>
+          <t>Правительство разрешает торговлю запчастями ...</t>
         </is>
       </c>
     </row>
@@ -2656,22 +2656,22 @@
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>контрабанда сайгачьих рогов</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>02 August 2022</t>
+          <t>31 July 2022</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
         <is>
-          <t>https://www.kt.kz/rus/crime/_1377937567.html</t>
+          <t>https://vk.com/wall-9029295</t>
         </is>
       </c>
       <c r="E82" s="4" t="inlineStr">
         <is>
-          <t>В Алматы извращенца, пытавшегося изнасиловать дочь ...</t>
+          <t>Европейской степи: записи сообщества | ВКонтакте</t>
         </is>
       </c>
     </row>
@@ -2683,22 +2683,22 @@
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз балобанов</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>02 August 2022</t>
+          <t>01 August 2022</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
         <is>
-          <t>https://alarmyk24.ru/news/992053/v-mid-soobschili-o-priznanii-ssha-v-sozdanii-itarmii-ukrainy-dlya-atak-na-rf.html</t>
+          <t>https://polpred.com/news?ns=1&amp;cnt=69&amp;cat_a=1</t>
         </is>
       </c>
       <c r="E83" s="4" t="inlineStr">
         <is>
-          <t>В МИД сообщили о признании США в создании «IT-армии ...</t>
+          <t>Новости. Казахстан - Polpred.com Обзор СМИ</t>
         </is>
       </c>
     </row>
@@ -2710,22 +2710,22 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабанда сайгачьих рогов</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>03 August 2022</t>
+          <t>02 August 2022</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>https://kazpravda.kz/</t>
+          <t>https://www.kt.kz/rus/crime/_1377937567.html</t>
         </is>
       </c>
       <c r="E84" s="4" t="inlineStr">
         <is>
-          <t>Новости Казахстана - свежие, актуальные, последние ...</t>
+          <t>В Алматы извращенца, пытавшегося изнасиловать дочь ...</t>
         </is>
       </c>
     </row>
@@ -2742,17 +2742,17 @@
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>03 August 2022</t>
+          <t>02 August 2022</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>https://xn--80ahclcogc6ci4h.xn--90anlfbebar6i.xn--p1ai/multimedia/photo/tags.htm?f=1&amp;blk=10407240&amp;objInBlock=24?</t>
+          <t>https://alarmyk24.ru/news/992053/v-mid-soobschili-o-priznanii-ssha-v-sozdanii-itarmii-ukrainy-dlya-atak-na-rf.html</t>
         </is>
       </c>
       <c r="E85" s="4" t="inlineStr">
         <is>
-          <t>Фото по теме - Мультимедиа</t>
+          <t>В МИД сообщили о признании США в создании «IT-армии ...</t>
         </is>
       </c>
     </row>
@@ -2769,17 +2769,17 @@
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>03 August 2022</t>
+          <t>02 August 2022</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>https://vecher.kz/bolshaya-chast-stikhiynikh-svalok-v-almati-stroitelnie-otkhodi</t>
+          <t>https://life-kirzhach.ru/</t>
         </is>
       </c>
       <c r="E86" s="4" t="inlineStr">
         <is>
-          <t>Большая часть стихийных свалок в Алматы</t>
+          <t>Новости г. Киржач</t>
         </is>
       </c>
     </row>
@@ -2791,22 +2791,22 @@
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>контрабандный вывоз степных черепах</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>04 August 2022</t>
+          <t>03 August 2022</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>https://coollib.net/b/585891-dzherald-darrell-tri-bileta-do-edvencher-pod-pologom-pyanogo-lesa-zemlya-shorohov/read</t>
+          <t>https://kazpravda.kz/</t>
         </is>
       </c>
       <c r="E87" s="4" t="inlineStr">
         <is>
-          <t>Три билета до Эдвенчер; Под пологом пьяного леса</t>
+          <t>Новости Казахстана - свежие, актуальные, последние ...</t>
         </is>
       </c>
     </row>
@@ -2818,22 +2818,22 @@
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>контрабандный вывоз степных черепах</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>05 August 2022</t>
+          <t>03 August 2022</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>https://freylit.ru/nwsteme/22.html</t>
+          <t>https://xn--80ahclcogc6ci4h.xn--90anlfbebar6i.xn--p1ai/multimedia/photo/tags.htm?f=1&amp;blk=10407240&amp;objInBlock=24?</t>
         </is>
       </c>
       <c r="E88" s="4" t="inlineStr">
         <is>
-          <t>Надёжные и достоверные новости в рубрике: Общество</t>
+          <t>Фото по теме - Мультимедиа</t>
         </is>
       </c>
     </row>
@@ -2845,22 +2845,22 @@
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>06 August 2022</t>
+          <t>03 August 2022</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>https://fresh-poc-portal.focus-entmt.com/amp/18-%D0%B1%D1%80%D0%B0%D0%BA%D0%BE%D0%BD%D1%8C%D0%B5%D1%80%D0%BE%D0%B2-%D0%B7%D0%B0%D0%B4%D0%B5%D1%80%D0%B6%D0%B0%D0%BB-%D0%9A%D0%9D%D0%91-%D0%B7%D0%B0-%D0%B2%D1%8B%D0%B2%D0%BE%D0%B7-%D1%80%D0%BE%D0%B3%D0%BE%D0%B2-%D1%81%D0%B0%D0%B9%D0%B3%D0%B8.xhtml</t>
+          <t>https://vecher.kz/bolshaya-chast-stikhiynikh-svalok-v-almati-stroitelnie-otkhodi</t>
         </is>
       </c>
       <c r="E89" s="4" t="inlineStr">
         <is>
-          <t>18 браконьеров задержал КНБ за вывоз рогов сайги</t>
+          <t>Большая часть стихийных свалок в Алматы</t>
         </is>
       </c>
     </row>
@@ -2872,22 +2872,238 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>08 August 2022</t>
+          <t>04 August 2022</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
         <is>
-          <t>https://mediazona.ca/news/2022/08/08/8-years/amp/</t>
+          <t>https://coollib.net/b/585891-dzherald-darrell-tri-bileta-do-edvencher-pod-pologom-pyanogo-lesa-zemlya-shorohov/read</t>
         </is>
       </c>
       <c r="E90" s="4" t="inlineStr">
         <is>
-          <t>Трое астанчан получили сроки до 8 лет колонии за ...</t>
+          <t>Три билета до Эдвенчер; Под пологом пьяного леса</t>
+        </is>
+      </c>
+    </row>
+    <row r="91" ht="40" customHeight="1">
+      <c r="A91" s="3" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B91" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C91" s="3" t="inlineStr">
+        <is>
+          <t>05 August 2022</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="inlineStr">
+        <is>
+          <t>https://freylit.ru/nwsteme/22.html</t>
+        </is>
+      </c>
+      <c r="E91" s="4" t="inlineStr">
+        <is>
+          <t>Надёжные и достоверные новости в рубрике: Общество</t>
+        </is>
+      </c>
+    </row>
+    <row r="92" ht="40" customHeight="1">
+      <c r="A92" s="3" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B92" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C92" s="3" t="inlineStr">
+        <is>
+          <t>06 August 2022</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="inlineStr">
+        <is>
+          <t>https://fresh-poc-portal.focus-entmt.com/amp/18-%D0%B1%D1%80%D0%B0%D0%BA%D0%BE%D0%BD%D1%8C%D0%B5%D1%80%D0%BE%D0%B2-%D0%B7%D0%B0%D0%B4%D0%B5%D1%80%D0%B6%D0%B0%D0%BB-%D0%9A%D0%9D%D0%91-%D0%B7%D0%B0-%D0%B2%D1%8B%D0%B2%D0%BE%D0%B7-%D1%80%D0%BE%D0%B3%D0%BE%D0%B2-%D1%81%D0%B0%D0%B9%D0%B3%D0%B8.xhtml</t>
+        </is>
+      </c>
+      <c r="E92" s="4" t="inlineStr">
+        <is>
+          <t>18 браконьеров задержал КНБ за вывоз рогов сайги</t>
+        </is>
+      </c>
+    </row>
+    <row r="93" ht="40" customHeight="1">
+      <c r="A93" s="3" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>10 August 2022</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="inlineStr">
+        <is>
+          <t>https://todaykhv.ru/upload/iblock/551/Vyazemskie-vesti-_31-ot-11.08.2022.pdf</t>
+        </is>
+      </c>
+      <c r="E93" s="4" t="inlineStr">
+        <is>
+          <t>11 августа 2022 гîäа - Хабаровский край сегодня</t>
+        </is>
+      </c>
+    </row>
+    <row r="94" ht="40" customHeight="1">
+      <c r="A94" s="3" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="inlineStr">
+        <is>
+          <t>10 August 2022</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="inlineStr">
+        <is>
+          <t>https://alarmyk24.ru/news/1035285/tamogenniki-v-nignem-novgorode-nashli-v-posylke-simvoliku-natsistskoj-germanii.html</t>
+        </is>
+      </c>
+      <c r="E94" s="4" t="inlineStr">
+        <is>
+          <t>Таможенники в Нижнем Новгороде нашли в посылке ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="95" ht="40" customHeight="1">
+      <c r="A95" s="3" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>11 August 2022</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="inlineStr">
+        <is>
+          <t>https://vpravda.ru/archive/201906/</t>
+        </is>
+      </c>
+      <c r="E95" s="4" t="inlineStr">
+        <is>
+          <t>Архив материалов: 11.08.2022 | Волгоградская Правда</t>
+        </is>
+      </c>
+    </row>
+    <row r="96" ht="40" customHeight="1">
+      <c r="A96" s="3" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="inlineStr">
+        <is>
+          <t>13 August 2022</t>
+        </is>
+      </c>
+      <c r="D96" s="3" t="inlineStr">
+        <is>
+          <t>https://rubrikator.org/items/serial-obruchalnoe-kolco_154601</t>
+        </is>
+      </c>
+      <c r="E96" s="4" t="inlineStr">
+        <is>
+          <t>Сериал "Обручальное кольцо" (2008-2012) - Rubrikator.org</t>
+        </is>
+      </c>
+    </row>
+    <row r="97" ht="40" customHeight="1">
+      <c r="A97" s="3" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
+        <is>
+          <t>15 August 2022</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="inlineStr">
+        <is>
+          <t>https://berkovich-zametki.com/Guestbook/guestbook.html</t>
+        </is>
+      </c>
+      <c r="E97" s="4" t="inlineStr">
+        <is>
+          <t>Гостевая книга - портал "Заметки по еврейской истории"</t>
+        </is>
+      </c>
+    </row>
+    <row r="98" ht="40" customHeight="1">
+      <c r="A98" s="3" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="inlineStr">
+        <is>
+          <t>15 August 2022</t>
+        </is>
+      </c>
+      <c r="D98" s="3" t="inlineStr">
+        <is>
+          <t>https://sibru.com/</t>
+        </is>
+      </c>
+      <c r="E98" s="4" t="inlineStr">
+        <is>
+          <t>Новости Сибири: SibRu.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add headers in requests
</commit_message>
<xml_diff>
--- a/news.xlsx
+++ b/news.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,22 +496,22 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>контрабанда сайгачьих рогов</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>12 October 2021</t>
+          <t>б/д</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t>https://ru.sputnik.kz/20211012/Artefakty-na-sotni-tysyach-dollarov-bivni-mamonta-pytalis-vyvezti-v-Kitay---video-18383890.html</t>
+          <t>https://www.9111.ru/%D0%BD%D0%B5%D0%B7%D0%BD%D0%B0%D1%87%D0%B8%D1%82%D0%B5%D0%BB%D1%8C%D0%BD%D0%B0%D1%8F_%D0%B4%D0%BE%D0%BB%D1%8F/</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>Бивни мамонта: артефакты пытались провезти в Китай</t>
+          <t>Незначительная доля - 269 советов адвокатов и юристов</t>
         </is>
       </c>
     </row>
@@ -523,22 +523,22 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>15 October 2021</t>
+          <t>б/д</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t>https://informburo.kz/novosti/dlya-borby-s-kontrabandoj-sokolov-balobanov-iz-kazahstana-net-normativov</t>
+          <t>http://xn----8sbfclc1aiptedbpu.xn--p1ai/obyavleniya/</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>Для борьбы с контрабандой соколов-балобанов в ...</t>
+          <t>Объявления | Администрация городского поселения ...</t>
         </is>
       </c>
     </row>
@@ -550,22 +550,22 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>контрабанда сайгачьих рогов</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>09 November 2021</t>
+          <t>12 October 2021</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>https://ria.ru/tag_zashhitazhivotnykh/</t>
+          <t>https://ru.sputnik.kz/20211012/Artefakty-na-sotni-tysyach-dollarov-bivni-mamonta-pytalis-vyvezti-v-Kitay---video-18383890.html</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>Защита животных - последние новости сегодня</t>
+          <t>Бивни мамонта: артефакты пытались провезти в Китай</t>
         </is>
       </c>
     </row>
@@ -582,17 +582,17 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>18 November 2021</t>
+          <t>15 October 2021</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>https://lifehacker.ru/zhivotnye-na-grani-vymiraniya/</t>
+          <t>https://informburo.kz/novosti/dlya-borby-s-kontrabandoj-sokolov-balobanov-iz-kazahstana-net-normativov</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>Животные на грани вымирания: 13 видов, которые могут ...</t>
+          <t>Для борьбы с контрабандой соколов-балобанов в ...</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>16 January 2022</t>
+          <t>09 November 2021</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>https://zakon.uchet.kz/rus/docs/K1400000226</t>
+          <t>https://ria.ru/tag_zashhitazhivotnykh/</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>Уголовный кодекс Республики Казахстан</t>
+          <t>Защита животных - последние новости сегодня</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>19 January 2022</t>
+          <t>18 November 2021</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>http://forum-rybakov.ru/outfit/kachestvennye-i-funkcionalnye-seti-rybolovnye-obespechat-uvlekatelnoe-provedenie-dosuga-na-beregu-lyubogo-vodoema.html</t>
+          <t>https://lifehacker.ru/zhivotnye-na-grani-vymiraniya/</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>Качественные и функциональные сети рыболовные ...</t>
+          <t>Животные на грани вымирания: 13 видов, которые могут ...</t>
         </is>
       </c>
     </row>
@@ -658,22 +658,22 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>контрабанда сайгачьих рогов</t>
+          <t>контрабанда рогов сайгака</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>05 March 2022</t>
+          <t>16 January 2022</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>https://traumlibrary.ru/book/gogol-pss14-09/gogol-pss14-09.html</t>
+          <t>https://zakon.uchet.kz/rus/docs/K1400000226</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>Николай Гоголь. Том 9. Наброски, конспекты, планы ...</t>
+          <t>Уголовный кодекс Республики Казахстан</t>
         </is>
       </c>
     </row>
@@ -690,17 +690,17 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>18 March 2022</t>
+          <t>19 January 2022</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>https://www.kt.kz/rus/reviews/v_luganskoy_oblasti_obnaruzheny_zastenki_natsistov_tornado_1377930908.html</t>
+          <t>http://forum-rybakov.ru/outfit/kachestvennye-i-funkcionalnye-seti-rybolovnye-obespechat-uvlekatelnoe-provedenie-dosuga-na-beregu-lyubogo-vodoema.html</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>В Луганской области обнаружены застенки нацистов ...</t>
+          <t>Качественные и функциональные сети рыболовные ...</t>
         </is>
       </c>
     </row>
@@ -717,17 +717,17 @@
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>19 May 2022</t>
+          <t>01 February 2022</t>
         </is>
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
-          <t>https://gazetavechorka.ru/content/article/list-by-hashtag?hashtag=kontrabanda</t>
+          <t>https://ru.sputnik.kz/20191113/roga-saigak-kazakhstan-russia-12023128.html</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>Новости по хештегу #контрабанда - Вечорка</t>
+          <t>Рога сайги на сумму $600 тысяч пытались вывезти из ...</t>
         </is>
       </c>
     </row>
@@ -739,22 +739,22 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>23 May 2022</t>
+          <t>01 February 2022</t>
         </is>
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>https://kaspyinfo.ru/tag/kontrabanda?page=1</t>
+          <t>https://ru.sputnik.kz/20190912/golub-sokol-siriytsy-kazakhstan-zaderzhanie-ohota-11509175.html</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>контрабанда. Новости - КаспийИнфо</t>
+          <t>Полсотни голубей в багажнике: сирийцев задержали за ...</t>
         </is>
       </c>
     </row>
@@ -766,22 +766,22 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>08 June 2022</t>
+          <t>07 February 2022</t>
         </is>
       </c>
       <c r="D12" s="4" t="inlineStr">
         <is>
-          <t>https://www.uralskweek.kz/2022/06/08/v-kazaxstane-xotyat-razreshit-otstrel-sajgakov/</t>
+          <t>https://24.kz/ru/news/incidents/item/526461-bolee-800-shtuk-rogov-sajgi-izyali-v-karagandinskoj-oblasti</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>Документ о разрешении отстрела сайгаков ... - Uralskweek.kz</t>
+          <t>Более 800 штук рогов сайги изъяли в Карагандинской ...</t>
         </is>
       </c>
     </row>
@@ -793,22 +793,22 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>контрабанда сайгачьих рогов</t>
+          <t>незаконный вывоз рогов сайгака</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>01 July 2022</t>
+          <t>07 February 2022</t>
         </is>
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>https://liter.kz/roga-saigakov-na-2-5-milliarda-pytalis-vyvezti-v-rossiiu-zhiteli-uralska-1656690447/</t>
+          <t>https://www.ohotniki.kz/articles/brakonerstvo/1727-svyshe-800-rogov-sajgi-nashli-v-salone-avto-v-karagandinskoj-oblasti</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>Рога сайгаков на 2,5 млрд пытались переправить в Россию ...</t>
+          <t>Свыше 800 рогов сайги нашли в салоне авто в ... - Ohotniki.kz</t>
         </is>
       </c>
     </row>
@@ -820,22 +820,22 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>контрабанда сайгачьих рогов</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>11 July 2022</t>
+          <t>25 February 2022</t>
         </is>
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>https://baigenews.kz/ekoduki_ekspert_saygaki_135167/</t>
+          <t>https://www.timacad.ru/uploads/files/20220225/1645798452_%D0%A1%D0%B1%D0%BE%D1%80%D0%BD%D0%B8%D0%BA%20%D1%82%D1%80%D1%83%D0%B4%D0%BE%D0%B2%20%D0%A1%D0%9C%D0%A3%D0%B8%D0%A1%202020%20%D0%B3.%20%D0%A2%D0%BE%D0%BC%202.pdf</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>"На Западе экодуки строят даже для червей". Эксперт о ...</t>
+          <t>Министерство сельского хозяйства - РГАУ-МСХА</t>
         </is>
       </c>
     </row>
@@ -852,17 +852,17 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>27 July 2022</t>
+          <t>02 March 2022</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>https://ru.sputnik.kg/20220727/kazahstan-roga-sajga-izyatie-1066348561.html</t>
+          <t>https://tsnik.kz/normativno-pravovye-akty/81097/</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>В Казахстане в машине нашли 2 000 рогов сайги</t>
+          <t>Уголовный кодекс Республики Казахстан 02.03.2022</t>
         </is>
       </c>
     </row>
@@ -879,17 +879,17 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>18 August 2022</t>
+          <t>02 March 2022</t>
         </is>
       </c>
       <c r="D16" s="4" t="inlineStr">
         <is>
-          <t>https://baigenews.kz/bolee-700-rogov-saygaka-izyali-u-brakonerov-v-karagandinskoy-oblasti_137193/</t>
+          <t>https://www.instagram.com/kursiv.media/</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>Более 700 рогов сайгака изъяли у ... - BaigeNews.kz</t>
+          <t>Курсив (@kursiv.media) • Instagram photos and videos</t>
         </is>
       </c>
     </row>
@@ -901,22 +901,22 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>20 August 2022</t>
+          <t>02 March 2022</t>
         </is>
       </c>
       <c r="D17" s="4" t="inlineStr">
         <is>
-          <t>https://ulysmedia.kz/news/11582-v-karagandinskoi-oblasti-prestupniki-zanimalis-nezakonnym-promyslom-krasnoknizhnykh-zhivotnykh/</t>
+          <t>https://nkvd.tomsk.ru/content/editor/KazakizaKamnem%202/20-Kazaki-za-Kamnem.pdf</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>Из Карагандинской пытались вывезти рога сайги на 15 млн ...</t>
+          <t>Казаки за Камнем - Следственная тюрьма НКВД</t>
         </is>
       </c>
     </row>
@@ -928,22 +928,22 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>контрабанда сайгачьих рогов</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>21 August 2022</t>
+          <t>05 March 2022</t>
         </is>
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
-          <t>https://liter.kz/roga-saigi-na-milliony-tenge-nelegalno-vezli-v-kitai-pomeshala-politsiia-karagandinskoi-oblasti-1661092819/</t>
+          <t>https://traumlibrary.ru/book/gogol-pss14-09/gogol-pss14-09.html</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
         <is>
-          <t>Вывезти в Китай рога сайги на миллионы тенге помешала ...</t>
+          <t>Николай Гоголь. Том 9. Наброски, конспекты, планы ...</t>
         </is>
       </c>
     </row>
@@ -960,17 +960,17 @@
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>21 August 2022</t>
+          <t>05 March 2022</t>
         </is>
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>https://www.zakon.kz/6022754-roga-saigi-na-15-mln-tenge-pytalis-vyvezti-iz-karagandinskoi-oblasti.html</t>
+          <t>https://www.kt.kz/rus/politics/rossiya_zakonchit_spetsoperatsiyu_na_ukraine_cherez_desyat_dney_1377930342.html</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>Рога сайги на 15 млн тенге пытались вывезти из ... - Zakon.kz</t>
+          <t>Американский военный эксперт спрогнозировал сроки ...</t>
         </is>
       </c>
     </row>
@@ -987,17 +987,17 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>21 August 2022</t>
+          <t>05 March 2022</t>
         </is>
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>https://kaztag.kz/ru/news/podozrevaemykh-v-popytke-sbyta-732-rogov-saygaka-v-kitay-zaderzhali-v-ulytau</t>
+          <t>https://blog-rk.ru/top/</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>Подозреваемых в попытке сбыта 732 рогов сайгака в ...</t>
+          <t>Архивы топ - Уютный Крым</t>
         </is>
       </c>
     </row>
@@ -1009,22 +1009,22 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>21 August 2022</t>
+          <t>05 March 2022</t>
         </is>
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
-          <t>https://newtimes.kz/proishestviya/155168-bolee-700-rogov-sajgaka-izyali-u-brakonerov-v-karagandinskoj-oblasti</t>
+          <t>https://raenza.ru/tags</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>Более 700 рогов сайгака изъяли у ... - NewTimes.kz</t>
+          <t>Все теги. Раёнза — новости Ново-Переделкино, Солнцево ...</t>
         </is>
       </c>
     </row>
@@ -1036,22 +1036,22 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>22 August 2022</t>
+          <t>05 March 2022</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>https://total.kz/ru/news/zhizn/bolee_700_rogov_saigaka_pitalis_perenapravit_v_kitai_date_2022_08_22_12_44_13</t>
+          <t>https://www.liveinternet.ru/users/lj_moskovitza/</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>Более 700 рогов сайгака пытались перенаправить в Китай</t>
+          <t>Московица Богородичный колпак - LiveInternet</t>
         </is>
       </c>
     </row>
@@ -1063,22 +1063,22 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>контрабанда рогов сайгака</t>
+          <t>незаконный вывоз балобанов</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>22 August 2022</t>
+          <t>05 March 2022</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>https://total.kz/ru/news/zhizn/bolee_700_rogov_saigaka_pitalis_perenapravit_v_kitai_date_2022_08_22_11_36_46</t>
+          <t>https://ru.djvu.online/file/bup05Tph2GOx0</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>Более 700 рогов сайги пытались перенаправить в Китай</t>
+          <t>ruski slownik. Верхнелужицко русский словарь - djvu.online</t>
         </is>
       </c>
     </row>
@@ -1090,22 +1090,22 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабандный вывоз степных черепах</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>22 August 2022</t>
+          <t>08 March 2022</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
-          <t>https://ru.sputnik.kz/20220822/bolee-700-shtuk-rogov-saygi-izyali-u-brakonerov-v-ulytauskoy-oblasti-26904342.html</t>
+          <t>https://huggingface.co/sberbank-ai/ruBert-base/resolve/main/vocab.txt</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>Более 700 штук рогов сайги изъяли у браконьеров в ...</t>
+          <t>vocab.txt - Hugging Face</t>
         </is>
       </c>
     </row>
@@ -1117,22 +1117,22 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>незаконный вывоз рогов сайгака</t>
+          <t>контрабанда рогов сайгака</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>22 August 2022</t>
+          <t>18 March 2022</t>
         </is>
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
-          <t>https://news.mail.ru/incident/52710298/</t>
+          <t>https://www.kt.kz/rus/reviews/v_luganskoy_oblasti_obnaruzheny_zastenki_natsistov_tornado_1377930908.html</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>Более 700 рогов сайгака изъяли у ... - Новости Mail.ru</t>
+          <t>В Луганской области обнаружены застенки нацистов ...</t>
         </is>
       </c>
     </row>
@@ -1149,17 +1149,17 @@
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>22 August 2022</t>
+          <t>29 March 2022</t>
         </is>
       </c>
       <c r="D26" s="4" t="inlineStr">
         <is>
-          <t>https://inbusiness.kz/ru/last/opg-po-dobyche-rogov-sajgi-neskolko-let-dejstvovala-v-karagandinskoj-i-ulytauskoj-oblastyah</t>
+          <t>https://zanmedia.kz/archives/70518</t>
         </is>
       </c>
       <c r="E26" s="4" t="inlineStr">
         <is>
-          <t>ОПГ по добыче рогов сайги несколько лет действовала в ...</t>
+          <t>Семь лет заключения за рога сайгаков | - ZANMEDIA.KZ</t>
         </is>
       </c>
     </row>
@@ -1176,17 +1176,17 @@
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>22 August 2022</t>
+          <t>10 April 2022</t>
         </is>
       </c>
       <c r="D27" s="4" t="inlineStr">
         <is>
-          <t>https://www.nur.kz/incident/crime/1984167-sotni-rogov-saygi-obnaruzhili-v-bagazhnike-avto-v-ulytau-tri-cheloveka-obyavleny-v-rozysk/</t>
+          <t>https://www.kt.kz/rus/economy/v_kazahstane_proizvoditeli_muki_priostanavlivayut_rabotu_1377931970.html</t>
         </is>
       </c>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>Сотни рогов сайги обнаружили в багажнике авто в Улытау ...</t>
+          <t>В Казахстане производители муки приостанавливают ...</t>
         </is>
       </c>
     </row>
@@ -1203,17 +1203,1475 @@
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
+          <t>11 April 2022</t>
+        </is>
+      </c>
+      <c r="D28" s="4" t="inlineStr">
+        <is>
+          <t>https://azh.kz/ru/news/view/84190</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
+          <t>Одинаково ли виноваты браконьеры и их «покупатели»?</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="40" customHeight="1">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>14 April 2022</t>
+        </is>
+      </c>
+      <c r="D29" s="4" t="inlineStr">
+        <is>
+          <t>https://www.stihi.in.ua/forumreclist.php?author=50790&amp;poem=756</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
+          <t>Лента комментариев - Украинский Портал Поэзии</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="40" customHeight="1">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>15 April 2022</t>
+        </is>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
+          <t>https://prospect.com.ru/news/2107145/kazahstan-otkazalsya-ot-sozdaniya-platformy-tsifrovogo-pravitelstva-so-sberom.html</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="inlineStr">
+        <is>
+          <t>Казахстан отказался от создания платформы цифрового ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="40" customHeight="1">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>26 April 2022</t>
+        </is>
+      </c>
+      <c r="D31" s="4" t="inlineStr">
+        <is>
+          <t>https://journal.tinkoff.ru/chita/</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="inlineStr">
+        <is>
+          <t>Жизнь в Чите</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="40" customHeight="1">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>06 May 2022</t>
+        </is>
+      </c>
+      <c r="D32" s="4" t="inlineStr">
+        <is>
+          <t>https://day-inews.ru/news/2237079/ne-dayut-zaputatsya-v-setyah-samarskie-obschestvenniki-spasayut-rybu-ot-brakonerov.html</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="inlineStr">
+        <is>
+          <t>Не дают запутаться в сетях: самарские общественники ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="40" customHeight="1">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>контрабандный вывоз степных черепах</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>12 May 2022</t>
+        </is>
+      </c>
+      <c r="D33" s="4" t="inlineStr">
+        <is>
+          <t>https://solaris-rio-zapchasti.ru/toyota/odomashnivanie-kakih-kakoe-zhivotnoe-chelovek-priruchil-pervym-varianty/</t>
+        </is>
+      </c>
+      <c r="E33" s="4" t="inlineStr">
+        <is>
+          <t>Одомашнивание каких. Какое животное человек приручил ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="40" customHeight="1">
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
+        <is>
+          <t>14 May 2022</t>
+        </is>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
+        <is>
+          <t>https://day-inews.ru/news/2255597/shojgu-zayavil-o-sozdanii-12-voinskih-chastej-v-otvet-na-rasshirenie-nato.html</t>
+        </is>
+      </c>
+      <c r="E34" s="4" t="inlineStr">
+        <is>
+          <t>Шойгу заявил о создании 12 воинских частей в ответ на ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="40" customHeight="1">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>15 May 2022</t>
+        </is>
+      </c>
+      <c r="D35" s="4" t="inlineStr">
+        <is>
+          <t>https://alarmyk24.ru/news/764605/ukraina-obstrelyala-belgorodskuyu-oblast.html</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
+          <t>Украина обстреляла Белгородскую область - alarmyk24.ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="40" customHeight="1">
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
+        <is>
+          <t>17 May 2022</t>
+        </is>
+      </c>
+      <c r="D36" s="4" t="inlineStr">
+        <is>
+          <t>http://duma.gov.ru/media/files/6BAKgQIvUzDZNPk2Gl8RALz1AL4crK9Q.pdf</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="inlineStr">
+        <is>
+          <t>ГОСУДАРСТВЕННАЯ ДУМА Стенограмма заседаний</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="40" customHeight="1">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="inlineStr">
+        <is>
+          <t>19 May 2022</t>
+        </is>
+      </c>
+      <c r="D37" s="4" t="inlineStr">
+        <is>
+          <t>https://gazetavechorka.ru/content/article/list-by-hashtag?hashtag=kontrabanda</t>
+        </is>
+      </c>
+      <c r="E37" s="4" t="inlineStr">
+        <is>
+          <t>Новости по хештегу #контрабанда - Вечорка</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="40" customHeight="1">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>19 May 2022</t>
+        </is>
+      </c>
+      <c r="D38" s="4" t="inlineStr">
+        <is>
+          <t>https://prospect.com.ru/news/2300649/kitaj-planiruet-zahvatit-kazahstan-plan-shelkovyj-put-vstupaet-v-silu.html</t>
+        </is>
+      </c>
+      <c r="E38" s="4" t="inlineStr">
+        <is>
+          <t>Шёлковый путь - Китай планирует захватить Казахстан</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="40" customHeight="1">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>23 May 2022</t>
+        </is>
+      </c>
+      <c r="D39" s="4" t="inlineStr">
+        <is>
+          <t>https://kaspyinfo.ru/tag/kontrabanda?page=1</t>
+        </is>
+      </c>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>контрабанда. Новости - КаспийИнфо</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="40" customHeight="1">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>24 May 2022</t>
+        </is>
+      </c>
+      <c r="D40" s="4" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/crime/5_1377934043.html</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
+          <t>Гражданин РК пытался незаконно вывезти из страны 5 ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="40" customHeight="1">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>25 May 2022</t>
+        </is>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>https://tnaneve.spb.ru/news/2899898/udar-v-spinu-kazahstan-predaet-rossiyu-i-ukreplyaet-strategicheskoe-partnerstvo-s-vashingtonom.html</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
+          <t>Удар в спину: Казахстан предает Россию и укрепляет ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="40" customHeight="1">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз балобанов</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>27 May 2022</t>
+        </is>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>https://www.tadviser.ru/index.php/%D0%A1%D1%82%D0%B0%D1%82%D1%8C%D1%8F:%D0%AD%D0%BB%D0%B5%D0%BA%D1%82%D1%80%D0%BE%D0%BD%D0%BD%D1%8B%D0%B5_%D0%B3%D0%BE%D1%81%D1%83%D1%81%D0%BB%D1%83%D0%B3%D0%B8</t>
+        </is>
+      </c>
+      <c r="E42" s="4" t="inlineStr">
+        <is>
+          <t>Электронные госуслуги - TAdviser</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="40" customHeight="1">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="inlineStr">
+        <is>
+          <t>08 June 2022</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="inlineStr">
+        <is>
+          <t>https://www.uralskweek.kz/2022/06/08/v-kazaxstane-xotyat-razreshit-otstrel-sajgakov/</t>
+        </is>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
+          <t>Документ о разрешении отстрела сайгаков ... - Uralskweek.kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="40" customHeight="1">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>01 July 2022</t>
+        </is>
+      </c>
+      <c r="D44" s="4" t="inlineStr">
+        <is>
+          <t>https://liter.kz/roga-saigakov-na-2-5-milliarda-pytalis-vyvezti-v-rossiiu-zhiteli-uralska-1656690447/</t>
+        </is>
+      </c>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
+          <t>Рога сайгаков на 2,5 млрд пытались переправить в Россию ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="40" customHeight="1">
+      <c r="A45" s="3" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="inlineStr">
+        <is>
+          <t>11 July 2022</t>
+        </is>
+      </c>
+      <c r="D45" s="4" t="inlineStr">
+        <is>
+          <t>https://baigenews.kz/ekoduki_ekspert_saygaki_135167/</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>"На Западе экодуки строят даже для червей". Эксперт о ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" ht="40" customHeight="1">
+      <c r="A46" s="3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>26 July 2022</t>
+        </is>
+      </c>
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>https://mediazona.ca/news/2022/07/26/saiga</t>
+        </is>
+      </c>
+      <c r="E46" s="4" t="inlineStr">
+        <is>
+          <t>Полиция Алматинской области изъяла у браконьеров 13 ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="40" customHeight="1">
+      <c r="A47" s="3" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>26 July 2022</t>
+        </is>
+      </c>
+      <c r="D47" s="4" t="inlineStr">
+        <is>
+          <t>https://www.inform.kz/ru/nezakonnuyu-ohotu-na-saygakov-vyyavili-v-kostanayskoy-oblasti_a3959179</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="inlineStr">
+        <is>
+          <t>Незаконную охоту на сайгаков выявили в Костанайской ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="40" customHeight="1">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>27 July 2022</t>
+        </is>
+      </c>
+      <c r="D48" s="4" t="inlineStr">
+        <is>
+          <t>https://ru.sputnik.kg/20220727/kazahstan-roga-sajga-izyatie-1066348561.html</t>
+        </is>
+      </c>
+      <c r="E48" s="4" t="inlineStr">
+        <is>
+          <t>В Казахстане в машине нашли 2 000 рогов сайги</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" ht="40" customHeight="1">
+      <c r="A49" s="3" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="inlineStr">
+        <is>
+          <t>30 July 2022</t>
+        </is>
+      </c>
+      <c r="D49" s="4" t="inlineStr">
+        <is>
+          <t>https://zonakz.net/2022/07/30/ceny-na-muku-i-luk-zamorozili-v-kostanajskoj-oblasti/</t>
+        </is>
+      </c>
+      <c r="E49" s="4" t="inlineStr">
+        <is>
+          <t>Цены на муку и лук заморозили в Костанайской области</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" ht="40" customHeight="1">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>02 August 2022</t>
+        </is>
+      </c>
+      <c r="D50" s="4" t="inlineStr">
+        <is>
+          <t>https://zonakz.net/2022/08/02/samolet-s-tretim-licom-ssha-prizemlilsya-v-tajvane-kitaj-protestuet/</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="inlineStr">
+        <is>
+          <t>Самолет с третьим лицом США приземлился в Тайване ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" ht="40" customHeight="1">
+      <c r="A51" s="3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="inlineStr">
+        <is>
+          <t>04 August 2022</t>
+        </is>
+      </c>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>https://gorvesti.ru/crime/pod-volgogradom-zaderzhali-parnya-vyraschivayuschego-doma-v-vedrakh-konoplyu-122105.html</t>
+        </is>
+      </c>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>Под Волгоградом задержали парня, выращивающего дома ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" ht="40" customHeight="1">
+      <c r="A52" s="3" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B52" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>05 August 2022</t>
+        </is>
+      </c>
+      <c r="D52" s="4" t="inlineStr">
+        <is>
+          <t>https://gorvesti.ru/accidents/pod-volgogradom-podrostok-zaderzhan-za-popytku-sbyt-krupnuyu-partiyu-narkotikov-122135.html</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="inlineStr">
+        <is>
+          <t>В Волгоградской области задержан 17-летний подросток ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" ht="40" customHeight="1">
+      <c r="A53" s="3" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>06 August 2022</t>
+        </is>
+      </c>
+      <c r="D53" s="4" t="inlineStr">
+        <is>
+          <t>https://fresh-poc-portal.focus-entmt.com/amp/18-%D0%B1%D1%80%D0%B0%D0%BA%D0%BE%D0%BD%D1%8C%D0%B5%D1%80%D0%BE%D0%B2-%D0%B7%D0%B0%D0%B4%D0%B5%D1%80%D0%B6%D0%B0%D0%BB-%D0%9A%D0%9D%D0%91-%D0%B7%D0%B0-%D0%B2%D1%8B%D0%B2%D0%BE%D0%B7-%D1%80%D0%BE%D0%B3%D0%BE%D0%B2-%D1%81%D0%B0%D0%B9%D0%B3%D0%B8.xhtml</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="inlineStr">
+        <is>
+          <t>18 браконьеров задержал КНБ за вывоз рогов сайги</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" ht="40" customHeight="1">
+      <c r="A54" s="3" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B54" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="inlineStr">
+        <is>
+          <t>10 August 2022</t>
+        </is>
+      </c>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>https://todaykhv.ru/upload/iblock/551/Vyazemskie-vesti-_31-ot-11.08.2022.pdf</t>
+        </is>
+      </c>
+      <c r="E54" s="4" t="inlineStr">
+        <is>
+          <t>11 августа 2022 гîäа - Хабаровский край сегодня</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" ht="40" customHeight="1">
+      <c r="A55" s="3" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="inlineStr">
+        <is>
+          <t>17 August 2022</t>
+        </is>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>https://visasam.ru/russia/tamozhnia/vvoz-v-uzbekistan.html</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>Таможенные правила и пошлины Узбекистана в 2022 году</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="40" customHeight="1">
+      <c r="A56" s="3" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="B56" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="inlineStr">
+        <is>
+          <t>18 August 2022</t>
+        </is>
+      </c>
+      <c r="D56" s="4" t="inlineStr">
+        <is>
+          <t>https://baigenews.kz/bolee-700-rogov-saygaka-izyali-u-brakonerov-v-karagandinskoy-oblasti_137193/</t>
+        </is>
+      </c>
+      <c r="E56" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 рогов сайгака изъяли у ... - BaigeNews.kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" ht="40" customHeight="1">
+      <c r="A57" s="3" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="B57" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C57" s="3" t="inlineStr">
+        <is>
+          <t>20 August 2022</t>
+        </is>
+      </c>
+      <c r="D57" s="4" t="inlineStr">
+        <is>
+          <t>https://ulysmedia.kz/news/11582-v-karagandinskoi-oblasti-prestupniki-zanimalis-nezakonnym-promyslom-krasnoknizhnykh-zhivotnykh/</t>
+        </is>
+      </c>
+      <c r="E57" s="4" t="inlineStr">
+        <is>
+          <t>Из Карагандинской пытались вывезти рога сайги на 15 млн ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="40" customHeight="1">
+      <c r="A58" s="3" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B58" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>https://liter.kz/roga-saigi-na-milliony-tenge-nelegalno-vezli-v-kitai-pomeshala-politsiia-karagandinskoi-oblasti-1661092819/</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>Вывезти в Китай рога сайги на миллионы тенге помешала ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" ht="40" customHeight="1">
+      <c r="A59" s="3" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D59" s="4" t="inlineStr">
+        <is>
+          <t>https://www.zakon.kz/6022754-roga-saigi-na-15-mln-tenge-pytalis-vyvezti-iz-karagandinskoi-oblasti.html</t>
+        </is>
+      </c>
+      <c r="E59" s="4" t="inlineStr">
+        <is>
+          <t>Рога сайги на 15 млн тенге пытались вывезти из ... - Zakon.kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" ht="40" customHeight="1">
+      <c r="A60" s="3" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C60" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D60" s="4" t="inlineStr">
+        <is>
+          <t>https://kaztag.kz/ru/news/podozrevaemykh-v-popytke-sbyta-732-rogov-saygaka-v-kitay-zaderzhali-v-ulytau</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>Подозреваемых в попытке сбыта 732 рогов сайгака в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" ht="40" customHeight="1">
+      <c r="A61" s="3" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B61" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C61" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D61" s="4" t="inlineStr">
+        <is>
+          <t>https://newtimes.kz/proishestviya/155168-bolee-700-rogov-sajgaka-izyali-u-brakonerov-v-karagandinskoj-oblasti</t>
+        </is>
+      </c>
+      <c r="E61" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 рогов сайгака изъяли у ... - NewTimes.kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="40" customHeight="1">
+      <c r="A62" s="3" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>https://kazakh24.info/7508-opg-brakonerov-s-bolee-700-rogov-saigakov-zaderzhana-v-ulytau-1661142046/</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
+        <is>
+          <t>ОПГ браконьеров с более 700 рогов сайгаков задержана в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="63" ht="40" customHeight="1">
+      <c r="A63" s="3" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="B63" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C63" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D63" s="4" t="inlineStr">
+        <is>
+          <t>https://orda.kz/bolee-700-rogov-sajgaka-izyali-policzejskie-v-ulytauskoj-oblasti/</t>
+        </is>
+      </c>
+      <c r="E63" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 рогов сайги изъяли полицейские в Улытауской ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="40" customHeight="1">
+      <c r="A64" s="3" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D64" s="4" t="inlineStr">
+        <is>
+          <t>https://kazlenta.kz/54481-150-kg-rogov-saygi-izyali-policeyskie-v-karagandinskoy-oblasti.html</t>
+        </is>
+      </c>
+      <c r="E64" s="4" t="inlineStr">
+        <is>
+          <t>150 кг рогов сайги изъяли полицейские в Карагандинской ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" ht="40" customHeight="1">
+      <c r="A65" s="3" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B65" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C65" s="3" t="inlineStr">
+        <is>
+          <t>21 August 2022</t>
+        </is>
+      </c>
+      <c r="D65" s="4" t="inlineStr">
+        <is>
+          <t>http://nv.kz/2022/08/21/275196/</t>
+        </is>
+      </c>
+      <c r="E65" s="4" t="inlineStr">
+        <is>
+          <t>Полицейские Карагандинской области изъяли более 700 ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="66" ht="40" customHeight="1">
+      <c r="A66" s="3" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B66" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C66" s="3" t="inlineStr">
+        <is>
           <t>22 August 2022</t>
         </is>
       </c>
-      <c r="D28" s="4" t="inlineStr">
-        <is>
-          <t>https://orda.kz/bolee-700-rogov-sajgaka-izyali-policzejskie-v-ulytauskoj-oblasti/</t>
-        </is>
-      </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>Более 700 рогов сайги изъяли полицейские в Улытауской ...</t>
+      <c r="D66" s="4" t="inlineStr">
+        <is>
+          <t>https://total.kz/ru/news/zhizn/bolee_700_rogov_saigaka_pitalis_perenapravit_v_kitai_date_2022_08_22_12_44_13</t>
+        </is>
+      </c>
+      <c r="E66" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 рогов сайгака пытались перенаправить в Китай</t>
+        </is>
+      </c>
+    </row>
+    <row r="67" ht="40" customHeight="1">
+      <c r="A67" s="3" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B67" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C67" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D67" s="4" t="inlineStr">
+        <is>
+          <t>https://total.kz/ru/news/zhizn/bolee_700_rogov_saigaka_pitalis_perenapravit_v_kitai_date_2022_08_22_11_36_46</t>
+        </is>
+      </c>
+      <c r="E67" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 рогов сайги пытались перенаправить в Китай</t>
+        </is>
+      </c>
+    </row>
+    <row r="68" ht="40" customHeight="1">
+      <c r="A68" s="3" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B68" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C68" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D68" s="4" t="inlineStr">
+        <is>
+          <t>https://ru.sputnik.kz/20220822/bolee-700-shtuk-rogov-saygi-izyali-u-brakonerov-v-ulytauskoy-oblasti-26904342.html</t>
+        </is>
+      </c>
+      <c r="E68" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 штук рогов сайги изъяли у браконьеров в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="69" ht="40" customHeight="1">
+      <c r="A69" s="3" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D69" s="4" t="inlineStr">
+        <is>
+          <t>https://news.mail.ru/incident/52710298/</t>
+        </is>
+      </c>
+      <c r="E69" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 рогов сайгака изъяли у ... - Новости Mail.ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="70" ht="40" customHeight="1">
+      <c r="A70" s="3" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C70" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D70" s="4" t="inlineStr">
+        <is>
+          <t>https://inbusiness.kz/ru/last/opg-po-dobyche-rogov-sajgi-neskolko-let-dejstvovala-v-karagandinskoj-i-ulytauskoj-oblastyah</t>
+        </is>
+      </c>
+      <c r="E70" s="4" t="inlineStr">
+        <is>
+          <t>ОПГ по добыче рогов сайги несколько лет действовала в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="71" ht="40" customHeight="1">
+      <c r="A71" s="3" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="B71" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C71" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D71" s="4" t="inlineStr">
+        <is>
+          <t>https://www.nur.kz/incident/crime/1984167-sotni-rogov-saygi-obnaruzhili-v-bagazhnike-avto-v-ulytau-tri-cheloveka-obyavleny-v-rozysk/</t>
+        </is>
+      </c>
+      <c r="E71" s="4" t="inlineStr">
+        <is>
+          <t>Сотни рогов сайги обнаружили в багажнике авто в Улытау ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="72" ht="40" customHeight="1">
+      <c r="A72" s="3" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D72" s="4" t="inlineStr">
+        <is>
+          <t>https://ohotniki.kz/articles/novosti/1991-bolee-700-rogov-sajgaka-iz-yali-u-brakonerov-v-karagandinskoj-oblasti</t>
+        </is>
+      </c>
+      <c r="E72" s="4" t="inlineStr">
+        <is>
+          <t>Более 700 рогов сайгака изъяли у браконьеров в ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="73" ht="40" customHeight="1">
+      <c r="A73" s="3" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B73" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C73" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D73" s="4" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/discover/%D0%BE%D1%82-%D1%82%D1%80%D0%B5%D1%85-%D0%B4%D0%BE-%D0%BF%D1%8F%D1%82%D0%B8-%D0%BB%D0%B5%D1%82</t>
+        </is>
+      </c>
+      <c r="E73" s="4" t="inlineStr">
+        <is>
+          <t>Descubre los videos populares de от трех до пяти лет - TikTok</t>
+        </is>
+      </c>
+    </row>
+    <row r="74" ht="40" customHeight="1">
+      <c r="A74" s="3" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B74" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D74" s="4" t="inlineStr">
+        <is>
+          <t>https://qansonar.com/news/1485-700-rogov-sajgi-iz-yali-u-brakonerov-v-karagandinskoj-oblasti</t>
+        </is>
+      </c>
+      <c r="E74" s="4" t="inlineStr">
+        <is>
+          <t>700 рогов сайги изъяли у браконьеров в Карагандинской ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="75" ht="40" customHeight="1">
+      <c r="A75" s="3" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B75" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C75" s="3" t="inlineStr">
+        <is>
+          <t>22 August 2022</t>
+        </is>
+      </c>
+      <c r="D75" s="4" t="inlineStr">
+        <is>
+          <t>https://polpred.com/news?ns=1&amp;cnt=69&amp;cat_a=1</t>
+        </is>
+      </c>
+      <c r="E75" s="4" t="inlineStr">
+        <is>
+          <t>Новости. Казахстан - Polpred.com Обзор СМИ</t>
+        </is>
+      </c>
+    </row>
+    <row r="76" ht="40" customHeight="1">
+      <c r="A76" s="3" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B76" s="3" t="inlineStr">
+        <is>
+          <t>контрабанда сайгачьих рогов</t>
+        </is>
+      </c>
+      <c r="C76" s="3" t="inlineStr">
+        <is>
+          <t>24 August 2022</t>
+        </is>
+      </c>
+      <c r="D76" s="4" t="inlineStr">
+        <is>
+          <t>https://inbusiness.kz/ru/last/pochti-200-shtuk-sajgachih-rogov-obnaruzhili-u-kazahstanca-emu-grozit-shtraf-ili-lishenie-svobody</t>
+        </is>
+      </c>
+      <c r="E76" s="4" t="inlineStr">
+        <is>
+          <t>Почти 200 штук сайгачьих рогов обнаружили у казахстанца</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" ht="40" customHeight="1">
+      <c r="A77" s="3" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="B77" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C77" s="3" t="inlineStr">
+        <is>
+          <t>24 August 2022</t>
+        </is>
+      </c>
+      <c r="D77" s="4" t="inlineStr">
+        <is>
+          <t>https://www.gov.kz/memleket/entities/mvd-karaganda/press/news/1</t>
+        </is>
+      </c>
+      <c r="E77" s="4" t="inlineStr">
+        <is>
+          <t>Логотип МВД РК - GOV.KZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="78" ht="40" customHeight="1">
+      <c r="A78" s="3" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="B78" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="inlineStr">
+        <is>
+          <t>25 August 2022</t>
+        </is>
+      </c>
+      <c r="D78" s="4" t="inlineStr">
+        <is>
+          <t>http://volgograd-news.net/incident/2022/08/25/246985.html</t>
+        </is>
+      </c>
+      <c r="E78" s="4" t="inlineStr">
+        <is>
+          <t>В Дзержинском районе Волгограда возле многоэтажки ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="79" ht="40" customHeight="1">
+      <c r="A79" s="3" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C79" s="3" t="inlineStr">
+        <is>
+          <t>25 August 2022</t>
+        </is>
+      </c>
+      <c r="D79" s="4" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/crime/knb_zavershil_rassledovanie_po_delu_masimova_i_ego_1377938672.html</t>
+        </is>
+      </c>
+      <c r="E79" s="4" t="inlineStr">
+        <is>
+          <t>КНБ завершил расследование по делу Масимова и его ...</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" ht="40" customHeight="1">
+      <c r="A80" s="3" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="B80" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C80" s="3" t="inlineStr">
+        <is>
+          <t>25 August 2022</t>
+        </is>
+      </c>
+      <c r="D80" s="4" t="inlineStr">
+        <is>
+          <t>https://vk.com/id340757700</t>
+        </is>
+      </c>
+      <c r="E80" s="4" t="inlineStr">
+        <is>
+          <t>Берик Жагипаров - ВКонтакте</t>
+        </is>
+      </c>
+    </row>
+    <row r="81" ht="40" customHeight="1">
+      <c r="A81" s="3" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="inlineStr">
+        <is>
+          <t>26 August 2022</t>
+        </is>
+      </c>
+      <c r="D81" s="4" t="inlineStr">
+        <is>
+          <t>https://www.kt.kz/rus/crime/_1377938697.html</t>
+        </is>
+      </c>
+      <c r="E81" s="4" t="inlineStr">
+        <is>
+          <t>В Талдыкоргане живодеры отрезали котенку уши</t>
+        </is>
+      </c>
+    </row>
+    <row r="82" ht="40" customHeight="1">
+      <c r="A82" s="3" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="B82" s="3" t="inlineStr">
+        <is>
+          <t>незаконный вывоз рогов сайгака</t>
+        </is>
+      </c>
+      <c r="C82" s="3" t="inlineStr">
+        <is>
+          <t>27 August 2022</t>
+        </is>
+      </c>
+      <c r="D82" s="4" t="inlineStr">
+        <is>
+          <t>https://www.inaktau.kz/news/cat/3</t>
+        </is>
+      </c>
+      <c r="E82" s="4" t="inlineStr">
+        <is>
+          <t>Общество - новости в Актау сегодня на inaktau.kz</t>
         </is>
       </c>
     </row>
@@ -1246,6 +2704,60 @@
     <hyperlink ref="D26" r:id="rId25"/>
     <hyperlink ref="D27" r:id="rId26"/>
     <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
+    <hyperlink ref="D46" r:id="rId45"/>
+    <hyperlink ref="D47" r:id="rId46"/>
+    <hyperlink ref="D48" r:id="rId47"/>
+    <hyperlink ref="D49" r:id="rId48"/>
+    <hyperlink ref="D50" r:id="rId49"/>
+    <hyperlink ref="D51" r:id="rId50"/>
+    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D53" r:id="rId52"/>
+    <hyperlink ref="D54" r:id="rId53"/>
+    <hyperlink ref="D55" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D57" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D59" r:id="rId58"/>
+    <hyperlink ref="D60" r:id="rId59"/>
+    <hyperlink ref="D61" r:id="rId60"/>
+    <hyperlink ref="D62" r:id="rId61"/>
+    <hyperlink ref="D63" r:id="rId62"/>
+    <hyperlink ref="D64" r:id="rId63"/>
+    <hyperlink ref="D65" r:id="rId64"/>
+    <hyperlink ref="D66" r:id="rId65"/>
+    <hyperlink ref="D67" r:id="rId66"/>
+    <hyperlink ref="D68" r:id="rId67"/>
+    <hyperlink ref="D69" r:id="rId68"/>
+    <hyperlink ref="D70" r:id="rId69"/>
+    <hyperlink ref="D71" r:id="rId70"/>
+    <hyperlink ref="D72" r:id="rId71"/>
+    <hyperlink ref="D73" r:id="rId72"/>
+    <hyperlink ref="D74" r:id="rId73"/>
+    <hyperlink ref="D75" r:id="rId74"/>
+    <hyperlink ref="D76" r:id="rId75"/>
+    <hyperlink ref="D77" r:id="rId76"/>
+    <hyperlink ref="D78" r:id="rId77"/>
+    <hyperlink ref="D79" r:id="rId78"/>
+    <hyperlink ref="D80" r:id="rId79"/>
+    <hyperlink ref="D81" r:id="rId80"/>
+    <hyperlink ref="D82" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>